<commit_message>
Major pages (sales, inventory and admin)
 - form validation
 - borrow
 - checkout
 - debtor service
 - added amount to cart model
</commit_message>
<xml_diff>
--- a/optimusinventory-api/sample inventory.xlsx
+++ b/optimusinventory-api/sample inventory.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E2">
         <v>50</v>

</xml_diff>